<commit_message>
refactoring for read test data from excel
</commit_message>
<xml_diff>
--- a/test-data/excel-data-provider.xlsx
+++ b/test-data/excel-data-provider.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/slava/git/playwright-page-object-example/test-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5C0F76C-96CA-8341-BC71-456A16510DBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B00C5C9F-A998-0C4D-8BAA-263424C7AD75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" xr2:uid="{2F752937-E091-7844-AF53-BF9599969C18}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>productToSearch</t>
   </si>
@@ -48,12 +48,6 @@
   </si>
   <si>
     <t>iphone 14 plus</t>
-  </si>
-  <si>
-    <t>7 items</t>
-  </si>
-  <si>
-    <t>39 items</t>
   </si>
 </sst>
 </file>
@@ -428,7 +422,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -453,8 +447,8 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
+      <c r="B2">
+        <v>7</v>
       </c>
       <c r="C2" s="1"/>
     </row>
@@ -462,8 +456,8 @@
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
+      <c r="B3">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>